<commit_message>
-Added in manual BP plot.
</commit_message>
<xml_diff>
--- a/BloodPressureDevice.xlsx
+++ b/BloodPressureDevice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\VitalsTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2592EFC8-D893-4696-B412-04FE9DE80B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A509C7B4-0AF6-4017-88F4-5DED3778724E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CF3A703-3A27-4153-A28D-24BD5F85AB0C}"/>
   </bookViews>
@@ -38,22 +38,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>DateTimeGroup (Local)</t>
+    <t>DateTimeGroup</t>
   </si>
   <si>
-    <t>SystolicBloodPressure(mmHG)</t>
+    <t>Systolic Blood Pressure (mmHG)</t>
   </si>
   <si>
-    <t>DiastolicBlood Pressure(mmHG)</t>
+    <t>Diastolic Blood Pressure (mmHG)</t>
   </si>
   <si>
-    <t>HeartRate(BPM)</t>
+    <t>Heart Rate (BPM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,10 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91ABE07-A005-41BF-BD7A-7513E29A11A9}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,16 +460,35 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="3">
+        <v>45143.754166666666</v>
+      </c>
+      <c r="B2" s="2">
+        <f>(128+125)/2</f>
+        <v>126.5</v>
+      </c>
+      <c r="C2" s="2">
+        <f>(91+88)/2</f>
+        <v>89.5</v>
+      </c>
+      <c r="D2" s="2">
+        <f>(84+88)/2</f>
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="3">
+        <v>45145.754166666666</v>
+      </c>
+      <c r="B3" s="2">
+        <v>123</v>
+      </c>
+      <c r="C3" s="2">
+        <v>80</v>
+      </c>
+      <c r="D3" s="2">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -634,6 +660,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Changed end date to system time as default. -Added in pulse oximeter data.
</commit_message>
<xml_diff>
--- a/BloodPressureDevice.xlsx
+++ b/BloodPressureDevice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\VitalsTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A509C7B4-0AF6-4017-88F4-5DED3778724E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94323A7-EE61-4B67-ABD1-3F491D436E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CF3A703-3A27-4153-A28D-24BD5F85AB0C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CF3A703-3A27-4153-A28D-24BD5F85AB0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>DateTimeGroup</t>
   </si>
@@ -49,6 +49,34 @@
   <si>
     <t>Heart Rate (BPM)</t>
   </si>
+  <si>
+    <r>
+      <t>Oxygen Saturation (% SpO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -57,7 +85,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +95,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,11 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +469,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,9 +481,10 @@
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +497,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45143.754166666666</v>
       </c>
@@ -475,188 +517,234 @@
         <f>(84+88)/2</f>
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>45145.754166666666</v>
+        <v>45144.576388888891</v>
       </c>
       <c r="B3" s="2">
+        <f>(125+121)/2</f>
         <v>123</v>
       </c>
       <c r="C3" s="2">
-        <v>80</v>
+        <f>(87+87)/2</f>
+        <v>87</v>
       </c>
       <c r="D3" s="2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+        <f>(104+94)/2</f>
+        <v>99</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>45144.799305555556</v>
+      </c>
+      <c r="B4" s="2">
+        <f>(125+125)/2</f>
+        <v>125</v>
+      </c>
+      <c r="C4" s="2">
+        <f>(88+88)/2</f>
+        <v>88</v>
+      </c>
+      <c r="D4" s="2">
+        <f>(89+89)/2</f>
+        <v>89</v>
+      </c>
+      <c r="E4" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
-Added new data. -Added Quarto document.
</commit_message>
<xml_diff>
--- a/BloodPressureDevice.xlsx
+++ b/BloodPressureDevice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\VitalsTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94323A7-EE61-4B67-ABD1-3F491D436E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B084DB58-C401-43FC-9F11-1482671282C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CF3A703-3A27-4153-A28D-24BD5F85AB0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CF3A703-3A27-4153-A28D-24BD5F85AB0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,12 +146,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +477,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +489,7 @@
     <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,254 +502,293 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>45143.754166666666</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <f>(128+125)/2</f>
         <v>126.5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <f>(91+88)/2</f>
         <v>89.5</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <f>(84+88)/2</f>
         <v>86</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>45144.576388888891</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <f>(125+121)/2</f>
         <v>123</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <f>(87+87)/2</f>
         <v>87</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <f>(104+94)/2</f>
         <v>99</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>45144.799305555556</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <f>(125+125)/2</f>
         <v>125</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <f>(88+88)/2</f>
         <v>88</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <f>(89+89)/2</f>
         <v>89</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="2">
+        <v>45145.527777777781</v>
+      </c>
+      <c r="B5" s="3">
+        <f>(137+134+127)/3</f>
+        <v>132.66666666666666</v>
+      </c>
+      <c r="C5" s="3">
+        <f>(100+93+89)/3</f>
+        <v>94</v>
+      </c>
+      <c r="D5" s="3">
+        <f>(100+94)/2</f>
+        <v>97</v>
+      </c>
+      <c r="E5" s="3">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="2">
+        <v>45146.59375</v>
+      </c>
+      <c r="B6" s="3">
+        <f>(130+125)/2</f>
+        <v>127.5</v>
+      </c>
+      <c r="C6" s="3">
+        <f>(91+89)/2</f>
+        <v>90</v>
+      </c>
+      <c r="D6" s="3">
+        <f>(91+98)/2</f>
+        <v>94.5</v>
+      </c>
+      <c r="E6" s="3">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="A7" s="2">
+        <v>45147.410416666666</v>
+      </c>
+      <c r="B7" s="3">
+        <f>(118+119)/2</f>
+        <v>118.5</v>
+      </c>
+      <c r="C7" s="3">
+        <f>(89+87)/2</f>
+        <v>88</v>
+      </c>
+      <c r="D7" s="3">
+        <f>(90+83)/2</f>
+        <v>86.5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
-Updated data. -Restricted graphs to display only five days of data.
</commit_message>
<xml_diff>
--- a/BloodPressureDevice.xlsx
+++ b/BloodPressureDevice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\VitalsTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B084DB58-C401-43FC-9F11-1482671282C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CE16AA-0F87-4B84-8E64-A80BDC1141AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CF3A703-3A27-4153-A28D-24BD5F85AB0C}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,25 +623,64 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="2">
+        <v>45148.472916666666</v>
+      </c>
+      <c r="B8" s="3">
+        <f>(123+126)/2</f>
+        <v>124.5</v>
+      </c>
+      <c r="C8" s="3">
+        <f>(81+85)/2</f>
+        <v>83</v>
+      </c>
+      <c r="D8" s="3">
+        <f>(95+89)/2</f>
+        <v>92</v>
+      </c>
+      <c r="E8" s="3">
+        <v>97</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="2">
+        <v>45148.597222222219</v>
+      </c>
+      <c r="B9" s="3">
+        <f>(130+124)/2</f>
+        <v>127</v>
+      </c>
+      <c r="C9" s="3">
+        <f>(90+88)/2</f>
+        <v>89</v>
+      </c>
+      <c r="D9" s="3">
+        <f>(89+86)/2</f>
+        <v>87.5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>98</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="2">
+        <v>45148.780555555553</v>
+      </c>
+      <c r="B10" s="3">
+        <f>(120+129)/2</f>
+        <v>124.5</v>
+      </c>
+      <c r="C10" s="3">
+        <f>(90+89)/2</f>
+        <v>89.5</v>
+      </c>
+      <c r="D10" s="3">
+        <f>(115+107)/2</f>
+        <v>111</v>
+      </c>
+      <c r="E10" s="3">
+        <v>95</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>

</xml_diff>

<commit_message>
-Updated data. -Added FitBit heart beat box plot.
</commit_message>
<xml_diff>
--- a/BloodPressureDevice.xlsx
+++ b/BloodPressureDevice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\VitalsTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B84325B-336B-4468-8FE3-38E8EC0B8DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8336C07-B9FD-47B6-A645-051F39A4D75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{0CF3A703-3A27-4153-A28D-24BD5F85AB0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CF3A703-3A27-4153-A28D-24BD5F85AB0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,18 +843,44 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="2">
+        <v>45156.743055555555</v>
+      </c>
+      <c r="B19" s="3">
+        <f>(134+128)/2</f>
+        <v>131</v>
+      </c>
+      <c r="C19" s="3">
+        <f>(94+89)/2</f>
+        <v>91.5</v>
+      </c>
+      <c r="D19" s="3">
+        <f>(85+78)/2</f>
+        <v>81.5</v>
+      </c>
+      <c r="E19" s="3">
+        <v>98</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="2">
+        <v>45157.40625</v>
+      </c>
+      <c r="B20" s="3">
+        <f>(129+136)/2</f>
+        <v>132.5</v>
+      </c>
+      <c r="C20" s="3">
+        <f>(91+93)/2</f>
+        <v>92</v>
+      </c>
+      <c r="D20" s="3">
+        <f>(97+103)/2</f>
+        <v>100</v>
+      </c>
+      <c r="E20" s="3">
+        <v>96</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>

</xml_diff>